<commit_message>
Fixed bugs in /people
</commit_message>
<xml_diff>
--- a/scripts/authors_generator/错误拼写纠正.xlsx
+++ b/scripts/authors_generator/错误拼写纠正.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文件\清华大学\0非课程\通班\Website\scripts\authors_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192C81AB-2001-453C-88B4-A96C634400C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45D8500-3EFA-403C-BFFB-73B7662A685C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -486,6 +486,9 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">

</xml_diff>